<commit_message>
V2 automatic script optimizing
</commit_message>
<xml_diff>
--- a/Controller Optimization/max_turn.xlsx
+++ b/Controller Optimization/max_turn.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inver\OneDrive\Desktop\PER 106\Simulation Conditions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inver\OneDrive\Desktop\Controller Optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E861D4D2-F8D5-4C4A-9533-5EF0909154D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3E80DC-961D-4FBD-9707-A7BDC61EFC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BF02C6E6-7C03-4F57-88F0-FD147FC419EC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>driver_input</t>
   </si>
@@ -52,18 +52,6 @@
   </si>
   <si>
     <t>wind z</t>
-  </si>
-  <si>
-    <t>b_FL</t>
-  </si>
-  <si>
-    <t>b_FR</t>
-  </si>
-  <si>
-    <t>b_RL</t>
-  </si>
-  <si>
-    <t>b_RR</t>
   </si>
   <si>
     <t>P_A</t>
@@ -424,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B44C769-8558-4087-85EA-24BCEBF1A080}">
-  <dimension ref="A1:M182"/>
+  <dimension ref="A1:I182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,7 +426,7 @@
     <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -446,13 +434,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -466,20 +454,8 @@
       <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -507,20 +483,8 @@
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -548,20 +512,8 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -589,20 +541,8 @@
       <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -630,20 +570,8 @@
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -671,20 +599,8 @@
       <c r="I6">
         <v>0</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -712,20 +628,8 @@
       <c r="I7">
         <v>0</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -753,20 +657,8 @@
       <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -794,20 +686,8 @@
       <c r="I9">
         <v>0</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -835,20 +715,8 @@
       <c r="I10">
         <v>0</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -876,20 +744,8 @@
       <c r="I11">
         <v>0</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -917,20 +773,8 @@
       <c r="I12">
         <v>0</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -958,20 +802,8 @@
       <c r="I13">
         <v>0</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -999,20 +831,8 @@
       <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1040,20 +860,8 @@
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1081,20 +889,8 @@
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1122,20 +918,8 @@
       <c r="I17">
         <v>0</v>
       </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1163,20 +947,8 @@
       <c r="I18">
         <v>0</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1204,20 +976,8 @@
       <c r="I19">
         <v>0</v>
       </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1245,20 +1005,8 @@
       <c r="I20">
         <v>0</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1286,20 +1034,8 @@
       <c r="I21">
         <v>0</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1327,20 +1063,8 @@
       <c r="I22">
         <v>0</v>
       </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1368,20 +1092,8 @@
       <c r="I23">
         <v>0</v>
       </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1409,20 +1121,8 @@
       <c r="I24">
         <v>0</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1450,20 +1150,8 @@
       <c r="I25">
         <v>0</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1491,20 +1179,8 @@
       <c r="I26">
         <v>0</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1532,20 +1208,8 @@
       <c r="I27">
         <v>0</v>
       </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1573,20 +1237,8 @@
       <c r="I28">
         <v>0</v>
       </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1614,20 +1266,8 @@
       <c r="I29">
         <v>0</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1655,20 +1295,8 @@
       <c r="I30">
         <v>0</v>
       </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1696,20 +1324,8 @@
       <c r="I31">
         <v>0</v>
       </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1737,20 +1353,8 @@
       <c r="I32">
         <v>0</v>
       </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1778,20 +1382,8 @@
       <c r="I33">
         <v>0</v>
       </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1819,20 +1411,8 @@
       <c r="I34">
         <v>0</v>
       </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
-      <c r="M34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1860,20 +1440,8 @@
       <c r="I35">
         <v>0</v>
       </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1901,20 +1469,8 @@
       <c r="I36">
         <v>0</v>
       </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1942,20 +1498,8 @@
       <c r="I37">
         <v>0</v>
       </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1983,20 +1527,8 @@
       <c r="I38">
         <v>0</v>
       </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2024,20 +1556,8 @@
       <c r="I39">
         <v>0</v>
       </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2065,20 +1585,8 @@
       <c r="I40">
         <v>0</v>
       </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2106,20 +1614,8 @@
       <c r="I41">
         <v>0</v>
       </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2147,20 +1643,8 @@
       <c r="I42">
         <v>0</v>
       </c>
-      <c r="J42">
-        <v>0</v>
-      </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2188,20 +1672,8 @@
       <c r="I43">
         <v>0</v>
       </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2229,20 +1701,8 @@
       <c r="I44">
         <v>0</v>
       </c>
-      <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-      <c r="L44">
-        <v>0</v>
-      </c>
-      <c r="M44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2270,20 +1730,8 @@
       <c r="I45">
         <v>0</v>
       </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-      <c r="M45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2311,20 +1759,8 @@
       <c r="I46">
         <v>0</v>
       </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
-      <c r="K46">
-        <v>0</v>
-      </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
-      <c r="M46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2352,20 +1788,8 @@
       <c r="I47">
         <v>0</v>
       </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-      <c r="L47">
-        <v>0</v>
-      </c>
-      <c r="M47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2393,20 +1817,8 @@
       <c r="I48">
         <v>0</v>
       </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="K48">
-        <v>0</v>
-      </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
-      <c r="M48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2434,20 +1846,8 @@
       <c r="I49">
         <v>0</v>
       </c>
-      <c r="J49">
-        <v>0</v>
-      </c>
-      <c r="K49">
-        <v>0</v>
-      </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-      <c r="M49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2475,20 +1875,8 @@
       <c r="I50">
         <v>0</v>
       </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <v>0</v>
-      </c>
-      <c r="L50">
-        <v>0</v>
-      </c>
-      <c r="M50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2516,20 +1904,8 @@
       <c r="I51">
         <v>0</v>
       </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
-      <c r="K51">
-        <v>0</v>
-      </c>
-      <c r="L51">
-        <v>0</v>
-      </c>
-      <c r="M51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2557,20 +1933,8 @@
       <c r="I52">
         <v>0</v>
       </c>
-      <c r="J52">
-        <v>0</v>
-      </c>
-      <c r="K52">
-        <v>0</v>
-      </c>
-      <c r="L52">
-        <v>0</v>
-      </c>
-      <c r="M52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2598,20 +1962,8 @@
       <c r="I53">
         <v>0</v>
       </c>
-      <c r="J53">
-        <v>0</v>
-      </c>
-      <c r="K53">
-        <v>0</v>
-      </c>
-      <c r="L53">
-        <v>0</v>
-      </c>
-      <c r="M53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2639,20 +1991,8 @@
       <c r="I54">
         <v>0</v>
       </c>
-      <c r="J54">
-        <v>0</v>
-      </c>
-      <c r="K54">
-        <v>0</v>
-      </c>
-      <c r="L54">
-        <v>0</v>
-      </c>
-      <c r="M54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2680,20 +2020,8 @@
       <c r="I55">
         <v>0</v>
       </c>
-      <c r="J55">
-        <v>0</v>
-      </c>
-      <c r="K55">
-        <v>0</v>
-      </c>
-      <c r="L55">
-        <v>0</v>
-      </c>
-      <c r="M55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2721,20 +2049,8 @@
       <c r="I56">
         <v>0</v>
       </c>
-      <c r="J56">
-        <v>0</v>
-      </c>
-      <c r="K56">
-        <v>0</v>
-      </c>
-      <c r="L56">
-        <v>0</v>
-      </c>
-      <c r="M56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2762,20 +2078,8 @@
       <c r="I57">
         <v>0</v>
       </c>
-      <c r="J57">
-        <v>0</v>
-      </c>
-      <c r="K57">
-        <v>0</v>
-      </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-      <c r="M57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2803,20 +2107,8 @@
       <c r="I58">
         <v>0</v>
       </c>
-      <c r="J58">
-        <v>0</v>
-      </c>
-      <c r="K58">
-        <v>0</v>
-      </c>
-      <c r="L58">
-        <v>0</v>
-      </c>
-      <c r="M58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2844,20 +2136,8 @@
       <c r="I59">
         <v>0</v>
       </c>
-      <c r="J59">
-        <v>0</v>
-      </c>
-      <c r="K59">
-        <v>0</v>
-      </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-      <c r="M59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2885,20 +2165,8 @@
       <c r="I60">
         <v>0</v>
       </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-      <c r="M60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2926,20 +2194,8 @@
       <c r="I61">
         <v>0</v>
       </c>
-      <c r="J61">
-        <v>0</v>
-      </c>
-      <c r="K61">
-        <v>0</v>
-      </c>
-      <c r="L61">
-        <v>0</v>
-      </c>
-      <c r="M61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2967,20 +2223,8 @@
       <c r="I62">
         <v>0</v>
       </c>
-      <c r="J62">
-        <v>0</v>
-      </c>
-      <c r="K62">
-        <v>0</v>
-      </c>
-      <c r="L62">
-        <v>0</v>
-      </c>
-      <c r="M62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3008,20 +2252,8 @@
       <c r="I63">
         <v>0</v>
       </c>
-      <c r="J63">
-        <v>0</v>
-      </c>
-      <c r="K63">
-        <v>0</v>
-      </c>
-      <c r="L63">
-        <v>0</v>
-      </c>
-      <c r="M63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3049,20 +2281,8 @@
       <c r="I64">
         <v>0</v>
       </c>
-      <c r="J64">
-        <v>0</v>
-      </c>
-      <c r="K64">
-        <v>0</v>
-      </c>
-      <c r="L64">
-        <v>0</v>
-      </c>
-      <c r="M64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3090,20 +2310,8 @@
       <c r="I65">
         <v>0</v>
       </c>
-      <c r="J65">
-        <v>0</v>
-      </c>
-      <c r="K65">
-        <v>0</v>
-      </c>
-      <c r="L65">
-        <v>0</v>
-      </c>
-      <c r="M65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3131,20 +2339,8 @@
       <c r="I66">
         <v>0</v>
       </c>
-      <c r="J66">
-        <v>0</v>
-      </c>
-      <c r="K66">
-        <v>0</v>
-      </c>
-      <c r="L66">
-        <v>0</v>
-      </c>
-      <c r="M66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3172,20 +2368,8 @@
       <c r="I67">
         <v>0</v>
       </c>
-      <c r="J67">
-        <v>0</v>
-      </c>
-      <c r="K67">
-        <v>0</v>
-      </c>
-      <c r="L67">
-        <v>0</v>
-      </c>
-      <c r="M67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3213,20 +2397,8 @@
       <c r="I68">
         <v>0</v>
       </c>
-      <c r="J68">
-        <v>0</v>
-      </c>
-      <c r="K68">
-        <v>0</v>
-      </c>
-      <c r="L68">
-        <v>0</v>
-      </c>
-      <c r="M68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3254,20 +2426,8 @@
       <c r="I69">
         <v>0</v>
       </c>
-      <c r="J69">
-        <v>0</v>
-      </c>
-      <c r="K69">
-        <v>0</v>
-      </c>
-      <c r="L69">
-        <v>0</v>
-      </c>
-      <c r="M69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3295,20 +2455,8 @@
       <c r="I70">
         <v>0</v>
       </c>
-      <c r="J70">
-        <v>0</v>
-      </c>
-      <c r="K70">
-        <v>0</v>
-      </c>
-      <c r="L70">
-        <v>0</v>
-      </c>
-      <c r="M70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3336,20 +2484,8 @@
       <c r="I71">
         <v>0</v>
       </c>
-      <c r="J71">
-        <v>0</v>
-      </c>
-      <c r="K71">
-        <v>0</v>
-      </c>
-      <c r="L71">
-        <v>0</v>
-      </c>
-      <c r="M71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3377,20 +2513,8 @@
       <c r="I72">
         <v>0</v>
       </c>
-      <c r="J72">
-        <v>0</v>
-      </c>
-      <c r="K72">
-        <v>0</v>
-      </c>
-      <c r="L72">
-        <v>0</v>
-      </c>
-      <c r="M72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3418,20 +2542,8 @@
       <c r="I73">
         <v>0</v>
       </c>
-      <c r="J73">
-        <v>0</v>
-      </c>
-      <c r="K73">
-        <v>0</v>
-      </c>
-      <c r="L73">
-        <v>0</v>
-      </c>
-      <c r="M73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3459,20 +2571,8 @@
       <c r="I74">
         <v>0</v>
       </c>
-      <c r="J74">
-        <v>0</v>
-      </c>
-      <c r="K74">
-        <v>0</v>
-      </c>
-      <c r="L74">
-        <v>0</v>
-      </c>
-      <c r="M74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3500,20 +2600,8 @@
       <c r="I75">
         <v>0</v>
       </c>
-      <c r="J75">
-        <v>0</v>
-      </c>
-      <c r="K75">
-        <v>0</v>
-      </c>
-      <c r="L75">
-        <v>0</v>
-      </c>
-      <c r="M75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3541,20 +2629,8 @@
       <c r="I76">
         <v>0</v>
       </c>
-      <c r="J76">
-        <v>0</v>
-      </c>
-      <c r="K76">
-        <v>0</v>
-      </c>
-      <c r="L76">
-        <v>0</v>
-      </c>
-      <c r="M76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3582,20 +2658,8 @@
       <c r="I77">
         <v>0</v>
       </c>
-      <c r="J77">
-        <v>0</v>
-      </c>
-      <c r="K77">
-        <v>0</v>
-      </c>
-      <c r="L77">
-        <v>0</v>
-      </c>
-      <c r="M77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3623,20 +2687,8 @@
       <c r="I78">
         <v>0</v>
       </c>
-      <c r="J78">
-        <v>0</v>
-      </c>
-      <c r="K78">
-        <v>0</v>
-      </c>
-      <c r="L78">
-        <v>0</v>
-      </c>
-      <c r="M78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -3664,20 +2716,8 @@
       <c r="I79">
         <v>0</v>
       </c>
-      <c r="J79">
-        <v>0</v>
-      </c>
-      <c r="K79">
-        <v>0</v>
-      </c>
-      <c r="L79">
-        <v>0</v>
-      </c>
-      <c r="M79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -3705,20 +2745,8 @@
       <c r="I80">
         <v>0</v>
       </c>
-      <c r="J80">
-        <v>0</v>
-      </c>
-      <c r="K80">
-        <v>0</v>
-      </c>
-      <c r="L80">
-        <v>0</v>
-      </c>
-      <c r="M80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3746,20 +2774,8 @@
       <c r="I81">
         <v>0</v>
       </c>
-      <c r="J81">
-        <v>0</v>
-      </c>
-      <c r="K81">
-        <v>0</v>
-      </c>
-      <c r="L81">
-        <v>0</v>
-      </c>
-      <c r="M81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -3787,20 +2803,8 @@
       <c r="I82">
         <v>0</v>
       </c>
-      <c r="J82">
-        <v>0</v>
-      </c>
-      <c r="K82">
-        <v>0</v>
-      </c>
-      <c r="L82">
-        <v>0</v>
-      </c>
-      <c r="M82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3828,20 +2832,8 @@
       <c r="I83">
         <v>0</v>
       </c>
-      <c r="J83">
-        <v>0</v>
-      </c>
-      <c r="K83">
-        <v>0</v>
-      </c>
-      <c r="L83">
-        <v>0</v>
-      </c>
-      <c r="M83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3869,20 +2861,8 @@
       <c r="I84">
         <v>0</v>
       </c>
-      <c r="J84">
-        <v>0</v>
-      </c>
-      <c r="K84">
-        <v>0</v>
-      </c>
-      <c r="L84">
-        <v>0</v>
-      </c>
-      <c r="M84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3910,20 +2890,8 @@
       <c r="I85">
         <v>0</v>
       </c>
-      <c r="J85">
-        <v>0</v>
-      </c>
-      <c r="K85">
-        <v>0</v>
-      </c>
-      <c r="L85">
-        <v>0</v>
-      </c>
-      <c r="M85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -3951,20 +2919,8 @@
       <c r="I86">
         <v>0</v>
       </c>
-      <c r="J86">
-        <v>0</v>
-      </c>
-      <c r="K86">
-        <v>0</v>
-      </c>
-      <c r="L86">
-        <v>0</v>
-      </c>
-      <c r="M86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -3992,20 +2948,8 @@
       <c r="I87">
         <v>0</v>
       </c>
-      <c r="J87">
-        <v>0</v>
-      </c>
-      <c r="K87">
-        <v>0</v>
-      </c>
-      <c r="L87">
-        <v>0</v>
-      </c>
-      <c r="M87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -4033,20 +2977,8 @@
       <c r="I88">
         <v>0</v>
       </c>
-      <c r="J88">
-        <v>0</v>
-      </c>
-      <c r="K88">
-        <v>0</v>
-      </c>
-      <c r="L88">
-        <v>0</v>
-      </c>
-      <c r="M88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -4074,20 +3006,8 @@
       <c r="I89">
         <v>0</v>
       </c>
-      <c r="J89">
-        <v>0</v>
-      </c>
-      <c r="K89">
-        <v>0</v>
-      </c>
-      <c r="L89">
-        <v>0</v>
-      </c>
-      <c r="M89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -4115,20 +3035,8 @@
       <c r="I90">
         <v>0</v>
       </c>
-      <c r="J90">
-        <v>0</v>
-      </c>
-      <c r="K90">
-        <v>0</v>
-      </c>
-      <c r="L90">
-        <v>0</v>
-      </c>
-      <c r="M90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -4156,20 +3064,8 @@
       <c r="I91">
         <v>0</v>
       </c>
-      <c r="J91">
-        <v>0</v>
-      </c>
-      <c r="K91">
-        <v>0</v>
-      </c>
-      <c r="L91">
-        <v>0</v>
-      </c>
-      <c r="M91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -4197,20 +3093,8 @@
       <c r="I92">
         <v>0</v>
       </c>
-      <c r="J92">
-        <v>0</v>
-      </c>
-      <c r="K92">
-        <v>0</v>
-      </c>
-      <c r="L92">
-        <v>0</v>
-      </c>
-      <c r="M92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -4238,20 +3122,8 @@
       <c r="I93">
         <v>0</v>
       </c>
-      <c r="J93">
-        <v>0</v>
-      </c>
-      <c r="K93">
-        <v>0</v>
-      </c>
-      <c r="L93">
-        <v>0</v>
-      </c>
-      <c r="M93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -4279,20 +3151,8 @@
       <c r="I94">
         <v>0</v>
       </c>
-      <c r="J94">
-        <v>0</v>
-      </c>
-      <c r="K94">
-        <v>0</v>
-      </c>
-      <c r="L94">
-        <v>0</v>
-      </c>
-      <c r="M94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
@@ -4320,20 +3180,8 @@
       <c r="I95">
         <v>0</v>
       </c>
-      <c r="J95">
-        <v>0</v>
-      </c>
-      <c r="K95">
-        <v>0</v>
-      </c>
-      <c r="L95">
-        <v>0</v>
-      </c>
-      <c r="M95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -4361,20 +3209,8 @@
       <c r="I96">
         <v>0</v>
       </c>
-      <c r="J96">
-        <v>0</v>
-      </c>
-      <c r="K96">
-        <v>0</v>
-      </c>
-      <c r="L96">
-        <v>0</v>
-      </c>
-      <c r="M96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
@@ -4402,20 +3238,8 @@
       <c r="I97">
         <v>0</v>
       </c>
-      <c r="J97">
-        <v>0</v>
-      </c>
-      <c r="K97">
-        <v>0</v>
-      </c>
-      <c r="L97">
-        <v>0</v>
-      </c>
-      <c r="M97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
@@ -4443,20 +3267,8 @@
       <c r="I98">
         <v>0</v>
       </c>
-      <c r="J98">
-        <v>0</v>
-      </c>
-      <c r="K98">
-        <v>0</v>
-      </c>
-      <c r="L98">
-        <v>0</v>
-      </c>
-      <c r="M98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
@@ -4484,20 +3296,8 @@
       <c r="I99">
         <v>0</v>
       </c>
-      <c r="J99">
-        <v>0</v>
-      </c>
-      <c r="K99">
-        <v>0</v>
-      </c>
-      <c r="L99">
-        <v>0</v>
-      </c>
-      <c r="M99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>98</v>
       </c>
@@ -4525,20 +3325,8 @@
       <c r="I100">
         <v>0</v>
       </c>
-      <c r="J100">
-        <v>0</v>
-      </c>
-      <c r="K100">
-        <v>0</v>
-      </c>
-      <c r="L100">
-        <v>0</v>
-      </c>
-      <c r="M100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>99</v>
       </c>
@@ -4566,20 +3354,8 @@
       <c r="I101">
         <v>0</v>
       </c>
-      <c r="J101">
-        <v>0</v>
-      </c>
-      <c r="K101">
-        <v>0</v>
-      </c>
-      <c r="L101">
-        <v>0</v>
-      </c>
-      <c r="M101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>100</v>
       </c>
@@ -4607,20 +3383,8 @@
       <c r="I102">
         <v>0</v>
       </c>
-      <c r="J102">
-        <v>0</v>
-      </c>
-      <c r="K102">
-        <v>0</v>
-      </c>
-      <c r="L102">
-        <v>0</v>
-      </c>
-      <c r="M102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>101</v>
       </c>
@@ -4648,20 +3412,8 @@
       <c r="I103">
         <v>0</v>
       </c>
-      <c r="J103">
-        <v>0</v>
-      </c>
-      <c r="K103">
-        <v>0</v>
-      </c>
-      <c r="L103">
-        <v>0</v>
-      </c>
-      <c r="M103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>102</v>
       </c>
@@ -4689,20 +3441,8 @@
       <c r="I104">
         <v>0</v>
       </c>
-      <c r="J104">
-        <v>0</v>
-      </c>
-      <c r="K104">
-        <v>0</v>
-      </c>
-      <c r="L104">
-        <v>0</v>
-      </c>
-      <c r="M104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>103</v>
       </c>
@@ -4730,20 +3470,8 @@
       <c r="I105">
         <v>0</v>
       </c>
-      <c r="J105">
-        <v>0</v>
-      </c>
-      <c r="K105">
-        <v>0</v>
-      </c>
-      <c r="L105">
-        <v>0</v>
-      </c>
-      <c r="M105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>104</v>
       </c>
@@ -4771,20 +3499,8 @@
       <c r="I106">
         <v>0</v>
       </c>
-      <c r="J106">
-        <v>0</v>
-      </c>
-      <c r="K106">
-        <v>0</v>
-      </c>
-      <c r="L106">
-        <v>0</v>
-      </c>
-      <c r="M106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>105</v>
       </c>
@@ -4812,20 +3528,8 @@
       <c r="I107">
         <v>0</v>
       </c>
-      <c r="J107">
-        <v>0</v>
-      </c>
-      <c r="K107">
-        <v>0</v>
-      </c>
-      <c r="L107">
-        <v>0</v>
-      </c>
-      <c r="M107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>106</v>
       </c>
@@ -4853,20 +3557,8 @@
       <c r="I108">
         <v>0</v>
       </c>
-      <c r="J108">
-        <v>0</v>
-      </c>
-      <c r="K108">
-        <v>0</v>
-      </c>
-      <c r="L108">
-        <v>0</v>
-      </c>
-      <c r="M108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>107</v>
       </c>
@@ -4894,20 +3586,8 @@
       <c r="I109">
         <v>0</v>
       </c>
-      <c r="J109">
-        <v>0</v>
-      </c>
-      <c r="K109">
-        <v>0</v>
-      </c>
-      <c r="L109">
-        <v>0</v>
-      </c>
-      <c r="M109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>108</v>
       </c>
@@ -4935,20 +3615,8 @@
       <c r="I110">
         <v>0</v>
       </c>
-      <c r="J110">
-        <v>0</v>
-      </c>
-      <c r="K110">
-        <v>0</v>
-      </c>
-      <c r="L110">
-        <v>0</v>
-      </c>
-      <c r="M110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>109</v>
       </c>
@@ -4976,20 +3644,8 @@
       <c r="I111">
         <v>0</v>
       </c>
-      <c r="J111">
-        <v>0</v>
-      </c>
-      <c r="K111">
-        <v>0</v>
-      </c>
-      <c r="L111">
-        <v>0</v>
-      </c>
-      <c r="M111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>110</v>
       </c>
@@ -5017,20 +3673,8 @@
       <c r="I112">
         <v>0</v>
       </c>
-      <c r="J112">
-        <v>0</v>
-      </c>
-      <c r="K112">
-        <v>0</v>
-      </c>
-      <c r="L112">
-        <v>0</v>
-      </c>
-      <c r="M112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>111</v>
       </c>
@@ -5058,20 +3702,8 @@
       <c r="I113">
         <v>0</v>
       </c>
-      <c r="J113">
-        <v>0</v>
-      </c>
-      <c r="K113">
-        <v>0</v>
-      </c>
-      <c r="L113">
-        <v>0</v>
-      </c>
-      <c r="M113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>112</v>
       </c>
@@ -5099,20 +3731,8 @@
       <c r="I114">
         <v>0</v>
       </c>
-      <c r="J114">
-        <v>0</v>
-      </c>
-      <c r="K114">
-        <v>0</v>
-      </c>
-      <c r="L114">
-        <v>0</v>
-      </c>
-      <c r="M114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>113</v>
       </c>
@@ -5140,20 +3760,8 @@
       <c r="I115">
         <v>0</v>
       </c>
-      <c r="J115">
-        <v>0</v>
-      </c>
-      <c r="K115">
-        <v>0</v>
-      </c>
-      <c r="L115">
-        <v>0</v>
-      </c>
-      <c r="M115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>114</v>
       </c>
@@ -5181,20 +3789,8 @@
       <c r="I116">
         <v>0</v>
       </c>
-      <c r="J116">
-        <v>0</v>
-      </c>
-      <c r="K116">
-        <v>0</v>
-      </c>
-      <c r="L116">
-        <v>0</v>
-      </c>
-      <c r="M116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>115</v>
       </c>
@@ -5222,20 +3818,8 @@
       <c r="I117">
         <v>0</v>
       </c>
-      <c r="J117">
-        <v>0</v>
-      </c>
-      <c r="K117">
-        <v>0</v>
-      </c>
-      <c r="L117">
-        <v>0</v>
-      </c>
-      <c r="M117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>116</v>
       </c>
@@ -5263,20 +3847,8 @@
       <c r="I118">
         <v>0</v>
       </c>
-      <c r="J118">
-        <v>0</v>
-      </c>
-      <c r="K118">
-        <v>0</v>
-      </c>
-      <c r="L118">
-        <v>0</v>
-      </c>
-      <c r="M118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>117</v>
       </c>
@@ -5304,20 +3876,8 @@
       <c r="I119">
         <v>0</v>
       </c>
-      <c r="J119">
-        <v>0</v>
-      </c>
-      <c r="K119">
-        <v>0</v>
-      </c>
-      <c r="L119">
-        <v>0</v>
-      </c>
-      <c r="M119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>118</v>
       </c>
@@ -5345,20 +3905,8 @@
       <c r="I120">
         <v>0</v>
       </c>
-      <c r="J120">
-        <v>0</v>
-      </c>
-      <c r="K120">
-        <v>0</v>
-      </c>
-      <c r="L120">
-        <v>0</v>
-      </c>
-      <c r="M120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>119</v>
       </c>
@@ -5386,20 +3934,8 @@
       <c r="I121">
         <v>0</v>
       </c>
-      <c r="J121">
-        <v>0</v>
-      </c>
-      <c r="K121">
-        <v>0</v>
-      </c>
-      <c r="L121">
-        <v>0</v>
-      </c>
-      <c r="M121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>120</v>
       </c>
@@ -5427,20 +3963,8 @@
       <c r="I122">
         <v>0</v>
       </c>
-      <c r="J122">
-        <v>0</v>
-      </c>
-      <c r="K122">
-        <v>0</v>
-      </c>
-      <c r="L122">
-        <v>0</v>
-      </c>
-      <c r="M122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>121</v>
       </c>
@@ -5468,20 +3992,8 @@
       <c r="I123">
         <v>0</v>
       </c>
-      <c r="J123">
-        <v>0</v>
-      </c>
-      <c r="K123">
-        <v>0</v>
-      </c>
-      <c r="L123">
-        <v>0</v>
-      </c>
-      <c r="M123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>122</v>
       </c>
@@ -5509,20 +4021,8 @@
       <c r="I124">
         <v>0</v>
       </c>
-      <c r="J124">
-        <v>0</v>
-      </c>
-      <c r="K124">
-        <v>0</v>
-      </c>
-      <c r="L124">
-        <v>0</v>
-      </c>
-      <c r="M124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>123</v>
       </c>
@@ -5550,20 +4050,8 @@
       <c r="I125">
         <v>0</v>
       </c>
-      <c r="J125">
-        <v>0</v>
-      </c>
-      <c r="K125">
-        <v>0</v>
-      </c>
-      <c r="L125">
-        <v>0</v>
-      </c>
-      <c r="M125">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>124</v>
       </c>
@@ -5591,20 +4079,8 @@
       <c r="I126">
         <v>0</v>
       </c>
-      <c r="J126">
-        <v>0</v>
-      </c>
-      <c r="K126">
-        <v>0</v>
-      </c>
-      <c r="L126">
-        <v>0</v>
-      </c>
-      <c r="M126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>125</v>
       </c>
@@ -5632,20 +4108,8 @@
       <c r="I127">
         <v>0</v>
       </c>
-      <c r="J127">
-        <v>0</v>
-      </c>
-      <c r="K127">
-        <v>0</v>
-      </c>
-      <c r="L127">
-        <v>0</v>
-      </c>
-      <c r="M127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>126</v>
       </c>
@@ -5673,20 +4137,8 @@
       <c r="I128">
         <v>0</v>
       </c>
-      <c r="J128">
-        <v>0</v>
-      </c>
-      <c r="K128">
-        <v>0</v>
-      </c>
-      <c r="L128">
-        <v>0</v>
-      </c>
-      <c r="M128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>127</v>
       </c>
@@ -5714,20 +4166,8 @@
       <c r="I129">
         <v>0</v>
       </c>
-      <c r="J129">
-        <v>0</v>
-      </c>
-      <c r="K129">
-        <v>0</v>
-      </c>
-      <c r="L129">
-        <v>0</v>
-      </c>
-      <c r="M129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>128</v>
       </c>
@@ -5755,20 +4195,8 @@
       <c r="I130">
         <v>0</v>
       </c>
-      <c r="J130">
-        <v>0</v>
-      </c>
-      <c r="K130">
-        <v>0</v>
-      </c>
-      <c r="L130">
-        <v>0</v>
-      </c>
-      <c r="M130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>129</v>
       </c>
@@ -5796,20 +4224,8 @@
       <c r="I131">
         <v>0</v>
       </c>
-      <c r="J131">
-        <v>0</v>
-      </c>
-      <c r="K131">
-        <v>0</v>
-      </c>
-      <c r="L131">
-        <v>0</v>
-      </c>
-      <c r="M131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>130</v>
       </c>
@@ -5837,20 +4253,8 @@
       <c r="I132">
         <v>0</v>
       </c>
-      <c r="J132">
-        <v>0</v>
-      </c>
-      <c r="K132">
-        <v>0</v>
-      </c>
-      <c r="L132">
-        <v>0</v>
-      </c>
-      <c r="M132">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>131</v>
       </c>
@@ -5878,20 +4282,8 @@
       <c r="I133">
         <v>0</v>
       </c>
-      <c r="J133">
-        <v>0</v>
-      </c>
-      <c r="K133">
-        <v>0</v>
-      </c>
-      <c r="L133">
-        <v>0</v>
-      </c>
-      <c r="M133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>132</v>
       </c>
@@ -5919,20 +4311,8 @@
       <c r="I134">
         <v>0</v>
       </c>
-      <c r="J134">
-        <v>0</v>
-      </c>
-      <c r="K134">
-        <v>0</v>
-      </c>
-      <c r="L134">
-        <v>0</v>
-      </c>
-      <c r="M134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>133</v>
       </c>
@@ -5960,20 +4340,8 @@
       <c r="I135">
         <v>0</v>
       </c>
-      <c r="J135">
-        <v>0</v>
-      </c>
-      <c r="K135">
-        <v>0</v>
-      </c>
-      <c r="L135">
-        <v>0</v>
-      </c>
-      <c r="M135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>134</v>
       </c>
@@ -6001,20 +4369,8 @@
       <c r="I136">
         <v>0</v>
       </c>
-      <c r="J136">
-        <v>0</v>
-      </c>
-      <c r="K136">
-        <v>0</v>
-      </c>
-      <c r="L136">
-        <v>0</v>
-      </c>
-      <c r="M136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>135</v>
       </c>
@@ -6042,20 +4398,8 @@
       <c r="I137">
         <v>0</v>
       </c>
-      <c r="J137">
-        <v>0</v>
-      </c>
-      <c r="K137">
-        <v>0</v>
-      </c>
-      <c r="L137">
-        <v>0</v>
-      </c>
-      <c r="M137">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>136</v>
       </c>
@@ -6083,20 +4427,8 @@
       <c r="I138">
         <v>0</v>
       </c>
-      <c r="J138">
-        <v>0</v>
-      </c>
-      <c r="K138">
-        <v>0</v>
-      </c>
-      <c r="L138">
-        <v>0</v>
-      </c>
-      <c r="M138">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>137</v>
       </c>
@@ -6124,20 +4456,8 @@
       <c r="I139">
         <v>0</v>
       </c>
-      <c r="J139">
-        <v>0</v>
-      </c>
-      <c r="K139">
-        <v>0</v>
-      </c>
-      <c r="L139">
-        <v>0</v>
-      </c>
-      <c r="M139">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>138</v>
       </c>
@@ -6165,20 +4485,8 @@
       <c r="I140">
         <v>0</v>
       </c>
-      <c r="J140">
-        <v>0</v>
-      </c>
-      <c r="K140">
-        <v>0</v>
-      </c>
-      <c r="L140">
-        <v>0</v>
-      </c>
-      <c r="M140">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>139</v>
       </c>
@@ -6206,20 +4514,8 @@
       <c r="I141">
         <v>0</v>
       </c>
-      <c r="J141">
-        <v>0</v>
-      </c>
-      <c r="K141">
-        <v>0</v>
-      </c>
-      <c r="L141">
-        <v>0</v>
-      </c>
-      <c r="M141">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>140</v>
       </c>
@@ -6247,20 +4543,8 @@
       <c r="I142">
         <v>0</v>
       </c>
-      <c r="J142">
-        <v>0</v>
-      </c>
-      <c r="K142">
-        <v>0</v>
-      </c>
-      <c r="L142">
-        <v>0</v>
-      </c>
-      <c r="M142">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>141</v>
       </c>
@@ -6288,20 +4572,8 @@
       <c r="I143">
         <v>0</v>
       </c>
-      <c r="J143">
-        <v>0</v>
-      </c>
-      <c r="K143">
-        <v>0</v>
-      </c>
-      <c r="L143">
-        <v>0</v>
-      </c>
-      <c r="M143">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>142</v>
       </c>
@@ -6329,20 +4601,8 @@
       <c r="I144">
         <v>0</v>
       </c>
-      <c r="J144">
-        <v>0</v>
-      </c>
-      <c r="K144">
-        <v>0</v>
-      </c>
-      <c r="L144">
-        <v>0</v>
-      </c>
-      <c r="M144">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>143</v>
       </c>
@@ -6370,20 +4630,8 @@
       <c r="I145">
         <v>0</v>
       </c>
-      <c r="J145">
-        <v>0</v>
-      </c>
-      <c r="K145">
-        <v>0</v>
-      </c>
-      <c r="L145">
-        <v>0</v>
-      </c>
-      <c r="M145">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>144</v>
       </c>
@@ -6411,20 +4659,8 @@
       <c r="I146">
         <v>0</v>
       </c>
-      <c r="J146">
-        <v>0</v>
-      </c>
-      <c r="K146">
-        <v>0</v>
-      </c>
-      <c r="L146">
-        <v>0</v>
-      </c>
-      <c r="M146">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>145</v>
       </c>
@@ -6452,20 +4688,8 @@
       <c r="I147">
         <v>0</v>
       </c>
-      <c r="J147">
-        <v>0</v>
-      </c>
-      <c r="K147">
-        <v>0</v>
-      </c>
-      <c r="L147">
-        <v>0</v>
-      </c>
-      <c r="M147">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>146</v>
       </c>
@@ -6493,20 +4717,8 @@
       <c r="I148">
         <v>0</v>
       </c>
-      <c r="J148">
-        <v>0</v>
-      </c>
-      <c r="K148">
-        <v>0</v>
-      </c>
-      <c r="L148">
-        <v>0</v>
-      </c>
-      <c r="M148">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>147</v>
       </c>
@@ -6534,20 +4746,8 @@
       <c r="I149">
         <v>0</v>
       </c>
-      <c r="J149">
-        <v>0</v>
-      </c>
-      <c r="K149">
-        <v>0</v>
-      </c>
-      <c r="L149">
-        <v>0</v>
-      </c>
-      <c r="M149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>148</v>
       </c>
@@ -6575,20 +4775,8 @@
       <c r="I150">
         <v>0</v>
       </c>
-      <c r="J150">
-        <v>0</v>
-      </c>
-      <c r="K150">
-        <v>0</v>
-      </c>
-      <c r="L150">
-        <v>0</v>
-      </c>
-      <c r="M150">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>149</v>
       </c>
@@ -6616,20 +4804,8 @@
       <c r="I151">
         <v>0</v>
       </c>
-      <c r="J151">
-        <v>0</v>
-      </c>
-      <c r="K151">
-        <v>0</v>
-      </c>
-      <c r="L151">
-        <v>0</v>
-      </c>
-      <c r="M151">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>150</v>
       </c>
@@ -6657,20 +4833,8 @@
       <c r="I152">
         <v>0</v>
       </c>
-      <c r="J152">
-        <v>0</v>
-      </c>
-      <c r="K152">
-        <v>0</v>
-      </c>
-      <c r="L152">
-        <v>0</v>
-      </c>
-      <c r="M152">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>151</v>
       </c>
@@ -6698,20 +4862,8 @@
       <c r="I153">
         <v>0</v>
       </c>
-      <c r="J153">
-        <v>0</v>
-      </c>
-      <c r="K153">
-        <v>0</v>
-      </c>
-      <c r="L153">
-        <v>0</v>
-      </c>
-      <c r="M153">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>152</v>
       </c>
@@ -6739,20 +4891,8 @@
       <c r="I154">
         <v>0</v>
       </c>
-      <c r="J154">
-        <v>0</v>
-      </c>
-      <c r="K154">
-        <v>0</v>
-      </c>
-      <c r="L154">
-        <v>0</v>
-      </c>
-      <c r="M154">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>153</v>
       </c>
@@ -6780,20 +4920,8 @@
       <c r="I155">
         <v>0</v>
       </c>
-      <c r="J155">
-        <v>0</v>
-      </c>
-      <c r="K155">
-        <v>0</v>
-      </c>
-      <c r="L155">
-        <v>0</v>
-      </c>
-      <c r="M155">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>154</v>
       </c>
@@ -6821,20 +4949,8 @@
       <c r="I156">
         <v>0</v>
       </c>
-      <c r="J156">
-        <v>0</v>
-      </c>
-      <c r="K156">
-        <v>0</v>
-      </c>
-      <c r="L156">
-        <v>0</v>
-      </c>
-      <c r="M156">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>155</v>
       </c>
@@ -6862,20 +4978,8 @@
       <c r="I157">
         <v>0</v>
       </c>
-      <c r="J157">
-        <v>0</v>
-      </c>
-      <c r="K157">
-        <v>0</v>
-      </c>
-      <c r="L157">
-        <v>0</v>
-      </c>
-      <c r="M157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>156</v>
       </c>
@@ -6903,20 +5007,8 @@
       <c r="I158">
         <v>0</v>
       </c>
-      <c r="J158">
-        <v>0</v>
-      </c>
-      <c r="K158">
-        <v>0</v>
-      </c>
-      <c r="L158">
-        <v>0</v>
-      </c>
-      <c r="M158">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>157</v>
       </c>
@@ -6944,20 +5036,8 @@
       <c r="I159">
         <v>0</v>
       </c>
-      <c r="J159">
-        <v>0</v>
-      </c>
-      <c r="K159">
-        <v>0</v>
-      </c>
-      <c r="L159">
-        <v>0</v>
-      </c>
-      <c r="M159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>158</v>
       </c>
@@ -6985,20 +5065,8 @@
       <c r="I160">
         <v>0</v>
       </c>
-      <c r="J160">
-        <v>0</v>
-      </c>
-      <c r="K160">
-        <v>0</v>
-      </c>
-      <c r="L160">
-        <v>0</v>
-      </c>
-      <c r="M160">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>159</v>
       </c>
@@ -7026,20 +5094,8 @@
       <c r="I161">
         <v>0</v>
       </c>
-      <c r="J161">
-        <v>0</v>
-      </c>
-      <c r="K161">
-        <v>0</v>
-      </c>
-      <c r="L161">
-        <v>0</v>
-      </c>
-      <c r="M161">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>160</v>
       </c>
@@ -7067,20 +5123,8 @@
       <c r="I162">
         <v>0</v>
       </c>
-      <c r="J162">
-        <v>0</v>
-      </c>
-      <c r="K162">
-        <v>0</v>
-      </c>
-      <c r="L162">
-        <v>0</v>
-      </c>
-      <c r="M162">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>161</v>
       </c>
@@ -7108,20 +5152,8 @@
       <c r="I163">
         <v>0</v>
       </c>
-      <c r="J163">
-        <v>0</v>
-      </c>
-      <c r="K163">
-        <v>0</v>
-      </c>
-      <c r="L163">
-        <v>0</v>
-      </c>
-      <c r="M163">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>162</v>
       </c>
@@ -7149,20 +5181,8 @@
       <c r="I164">
         <v>0</v>
       </c>
-      <c r="J164">
-        <v>0</v>
-      </c>
-      <c r="K164">
-        <v>0</v>
-      </c>
-      <c r="L164">
-        <v>0</v>
-      </c>
-      <c r="M164">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>163</v>
       </c>
@@ -7190,20 +5210,8 @@
       <c r="I165">
         <v>0</v>
       </c>
-      <c r="J165">
-        <v>0</v>
-      </c>
-      <c r="K165">
-        <v>0</v>
-      </c>
-      <c r="L165">
-        <v>0</v>
-      </c>
-      <c r="M165">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>164</v>
       </c>
@@ -7231,20 +5239,8 @@
       <c r="I166">
         <v>0</v>
       </c>
-      <c r="J166">
-        <v>0</v>
-      </c>
-      <c r="K166">
-        <v>0</v>
-      </c>
-      <c r="L166">
-        <v>0</v>
-      </c>
-      <c r="M166">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>165</v>
       </c>
@@ -7272,20 +5268,8 @@
       <c r="I167">
         <v>0</v>
       </c>
-      <c r="J167">
-        <v>0</v>
-      </c>
-      <c r="K167">
-        <v>0</v>
-      </c>
-      <c r="L167">
-        <v>0</v>
-      </c>
-      <c r="M167">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>166</v>
       </c>
@@ -7313,20 +5297,8 @@
       <c r="I168">
         <v>0</v>
       </c>
-      <c r="J168">
-        <v>0</v>
-      </c>
-      <c r="K168">
-        <v>0</v>
-      </c>
-      <c r="L168">
-        <v>0</v>
-      </c>
-      <c r="M168">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>167</v>
       </c>
@@ -7354,20 +5326,8 @@
       <c r="I169">
         <v>0</v>
       </c>
-      <c r="J169">
-        <v>0</v>
-      </c>
-      <c r="K169">
-        <v>0</v>
-      </c>
-      <c r="L169">
-        <v>0</v>
-      </c>
-      <c r="M169">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>168</v>
       </c>
@@ -7395,20 +5355,8 @@
       <c r="I170">
         <v>0</v>
       </c>
-      <c r="J170">
-        <v>0</v>
-      </c>
-      <c r="K170">
-        <v>0</v>
-      </c>
-      <c r="L170">
-        <v>0</v>
-      </c>
-      <c r="M170">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>169</v>
       </c>
@@ -7436,20 +5384,8 @@
       <c r="I171">
         <v>0</v>
       </c>
-      <c r="J171">
-        <v>0</v>
-      </c>
-      <c r="K171">
-        <v>0</v>
-      </c>
-      <c r="L171">
-        <v>0</v>
-      </c>
-      <c r="M171">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>170</v>
       </c>
@@ -7477,20 +5413,8 @@
       <c r="I172">
         <v>0</v>
       </c>
-      <c r="J172">
-        <v>0</v>
-      </c>
-      <c r="K172">
-        <v>0</v>
-      </c>
-      <c r="L172">
-        <v>0</v>
-      </c>
-      <c r="M172">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>171</v>
       </c>
@@ -7518,20 +5442,8 @@
       <c r="I173">
         <v>0</v>
       </c>
-      <c r="J173">
-        <v>0</v>
-      </c>
-      <c r="K173">
-        <v>0</v>
-      </c>
-      <c r="L173">
-        <v>0</v>
-      </c>
-      <c r="M173">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>172</v>
       </c>
@@ -7559,20 +5471,8 @@
       <c r="I174">
         <v>0</v>
       </c>
-      <c r="J174">
-        <v>0</v>
-      </c>
-      <c r="K174">
-        <v>0</v>
-      </c>
-      <c r="L174">
-        <v>0</v>
-      </c>
-      <c r="M174">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>173</v>
       </c>
@@ -7600,20 +5500,8 @@
       <c r="I175">
         <v>0</v>
       </c>
-      <c r="J175">
-        <v>0</v>
-      </c>
-      <c r="K175">
-        <v>0</v>
-      </c>
-      <c r="L175">
-        <v>0</v>
-      </c>
-      <c r="M175">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>174</v>
       </c>
@@ -7641,20 +5529,8 @@
       <c r="I176">
         <v>0</v>
       </c>
-      <c r="J176">
-        <v>0</v>
-      </c>
-      <c r="K176">
-        <v>0</v>
-      </c>
-      <c r="L176">
-        <v>0</v>
-      </c>
-      <c r="M176">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>175</v>
       </c>
@@ -7682,20 +5558,8 @@
       <c r="I177">
         <v>0</v>
       </c>
-      <c r="J177">
-        <v>0</v>
-      </c>
-      <c r="K177">
-        <v>0</v>
-      </c>
-      <c r="L177">
-        <v>0</v>
-      </c>
-      <c r="M177">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>176</v>
       </c>
@@ -7723,20 +5587,8 @@
       <c r="I178">
         <v>0</v>
       </c>
-      <c r="J178">
-        <v>0</v>
-      </c>
-      <c r="K178">
-        <v>0</v>
-      </c>
-      <c r="L178">
-        <v>0</v>
-      </c>
-      <c r="M178">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>177</v>
       </c>
@@ -7764,20 +5616,8 @@
       <c r="I179">
         <v>0</v>
       </c>
-      <c r="J179">
-        <v>0</v>
-      </c>
-      <c r="K179">
-        <v>0</v>
-      </c>
-      <c r="L179">
-        <v>0</v>
-      </c>
-      <c r="M179">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>178</v>
       </c>
@@ -7805,20 +5645,8 @@
       <c r="I180">
         <v>0</v>
       </c>
-      <c r="J180">
-        <v>0</v>
-      </c>
-      <c r="K180">
-        <v>0</v>
-      </c>
-      <c r="L180">
-        <v>0</v>
-      </c>
-      <c r="M180">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>179</v>
       </c>
@@ -7846,20 +5674,8 @@
       <c r="I181">
         <v>0</v>
       </c>
-      <c r="J181">
-        <v>0</v>
-      </c>
-      <c r="K181">
-        <v>0</v>
-      </c>
-      <c r="L181">
-        <v>0</v>
-      </c>
-      <c r="M181">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>180</v>
       </c>
@@ -7885,18 +5701,6 @@
         <v>0</v>
       </c>
       <c r="I182">
-        <v>0</v>
-      </c>
-      <c r="J182">
-        <v>0</v>
-      </c>
-      <c r="K182">
-        <v>0</v>
-      </c>
-      <c r="L182">
-        <v>0</v>
-      </c>
-      <c r="M182">
         <v>0</v>
       </c>
     </row>

</xml_diff>